<commit_message>
Fully completed gear selection based on recommended spur gears and cost on HPC. Efficiency is slightly odd.
</commit_message>
<xml_diff>
--- a/Gear Selection/Strength Factor.xlsx
+++ b/Gear Selection/Strength Factor.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William\Documents\Imperial\DMT\Technical Data\Helical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William\Documents\Imperial\Coop-robolift\Gear Selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13452" windowHeight="7728" activeTab="1" xr2:uid="{C2DD2191-E7E1-49AF-83C6-649F4D4705C0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13452" windowHeight="7728" activeTab="2" xr2:uid="{C2DD2191-E7E1-49AF-83C6-649F4D4705C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Z 1745 d" sheetId="1" r:id="rId1"/>
-    <sheet name="Y" sheetId="2" r:id="rId2"/>
+    <sheet name="Y Helic" sheetId="2" r:id="rId2"/>
+    <sheet name="Y Spur" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D3EA0D-CF60-4EF0-A00A-2DBDFD13D29E}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection sqref="A1:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1191,59 +1191,59 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <f>'Z 1745 d'!B2*Y!$C$18</f>
+        <f>'Z 1745 d'!B2*'Y Helic'!$C$18</f>
         <v>2.3516999999999997</v>
       </c>
       <c r="C2">
-        <f>'Z 1745 d'!C2*Y!$C$18</f>
+        <f>'Z 1745 d'!C2*'Y Helic'!$C$18</f>
         <v>2.26728</v>
       </c>
       <c r="D2">
-        <f>'Z 1745 d'!D2*Y!$C$18</f>
+        <f>'Z 1745 d'!D2*'Y Helic'!$C$18</f>
         <v>2.2311000000000001</v>
       </c>
       <c r="E2">
-        <f>'Z 1745 d'!E2*Y!$C$18</f>
+        <f>'Z 1745 d'!E2*'Y Helic'!$C$18</f>
         <v>2.12256</v>
       </c>
       <c r="F2">
-        <f>'Z 1745 d'!F2*Y!$C$18</f>
+        <f>'Z 1745 d'!F2*'Y Helic'!$C$18</f>
         <v>2.0984400000000001</v>
       </c>
       <c r="G2">
-        <f>'Z 1745 d'!G2*Y!$C$18</f>
+        <f>'Z 1745 d'!G2*'Y Helic'!$C$18</f>
         <v>1.9778399999999998</v>
       </c>
       <c r="H2">
-        <f>'Z 1745 d'!H2*Y!$C$18</f>
+        <f>'Z 1745 d'!H2*'Y Helic'!$C$18</f>
         <v>1.9054800000000001</v>
       </c>
       <c r="I2">
-        <f>'Z 1745 d'!I2*Y!$C$18</f>
+        <f>'Z 1745 d'!I2*'Y Helic'!$C$18</f>
         <v>1.8089999999999999</v>
       </c>
       <c r="J2">
-        <f>'Z 1745 d'!J2*Y!$C$18</f>
+        <f>'Z 1745 d'!J2*'Y Helic'!$C$18</f>
         <v>1.7486999999999999</v>
       </c>
       <c r="K2">
-        <f>'Z 1745 d'!K2*Y!$C$18</f>
+        <f>'Z 1745 d'!K2*'Y Helic'!$C$18</f>
         <v>1.6883999999999999</v>
       </c>
       <c r="L2">
-        <f>'Z 1745 d'!L2*Y!$C$18</f>
+        <f>'Z 1745 d'!L2*'Y Helic'!$C$18</f>
         <v>1.5557399999999999</v>
       </c>
       <c r="M2">
-        <f>'Z 1745 d'!M2*Y!$C$18</f>
+        <f>'Z 1745 d'!M2*'Y Helic'!$C$18</f>
         <v>1.4230799999999999</v>
       </c>
       <c r="N2">
-        <f>'Z 1745 d'!N2*Y!$C$18</f>
+        <f>'Z 1745 d'!N2*'Y Helic'!$C$18</f>
         <v>1.31454</v>
       </c>
       <c r="O2">
-        <f>'Z 1745 d'!O2*Y!$C$18</f>
+        <f>'Z 1745 d'!O2*'Y Helic'!$C$18</f>
         <v>1.206</v>
       </c>
     </row>
@@ -1253,59 +1253,59 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <f>'Z 1745 d'!B3*Y!$C$18</f>
+        <f>'Z 1745 d'!B3*'Y Helic'!$C$18</f>
         <v>2.7255599999999998</v>
       </c>
       <c r="C3">
-        <f>'Z 1745 d'!C3*Y!$C$18</f>
+        <f>'Z 1745 d'!C3*'Y Helic'!$C$18</f>
         <v>2.64114</v>
       </c>
       <c r="D3">
-        <f>'Z 1745 d'!D3*Y!$C$18</f>
+        <f>'Z 1745 d'!D3*'Y Helic'!$C$18</f>
         <v>2.6049600000000002</v>
       </c>
       <c r="E3">
-        <f>'Z 1745 d'!E3*Y!$C$18</f>
+        <f>'Z 1745 d'!E3*'Y Helic'!$C$18</f>
         <v>2.4843600000000001</v>
       </c>
       <c r="F3">
-        <f>'Z 1745 d'!F3*Y!$C$18</f>
+        <f>'Z 1745 d'!F3*'Y Helic'!$C$18</f>
         <v>2.39994</v>
       </c>
       <c r="G3">
-        <f>'Z 1745 d'!G3*Y!$C$18</f>
+        <f>'Z 1745 d'!G3*'Y Helic'!$C$18</f>
         <v>2.2793399999999999</v>
       </c>
       <c r="H3">
-        <f>'Z 1745 d'!H3*Y!$C$18</f>
+        <f>'Z 1745 d'!H3*'Y Helic'!$C$18</f>
         <v>2.1828599999999998</v>
       </c>
       <c r="I3">
-        <f>'Z 1745 d'!I3*Y!$C$18</f>
+        <f>'Z 1745 d'!I3*'Y Helic'!$C$18</f>
         <v>2.0622599999999998</v>
       </c>
       <c r="J3">
-        <f>'Z 1745 d'!J3*Y!$C$18</f>
+        <f>'Z 1745 d'!J3*'Y Helic'!$C$18</f>
         <v>1.9416600000000002</v>
       </c>
       <c r="K3">
-        <f>'Z 1745 d'!K3*Y!$C$18</f>
+        <f>'Z 1745 d'!K3*'Y Helic'!$C$18</f>
         <v>1.8693</v>
       </c>
       <c r="L3">
-        <f>'Z 1745 d'!L3*Y!$C$18</f>
+        <f>'Z 1745 d'!L3*'Y Helic'!$C$18</f>
         <v>1.73664</v>
       </c>
       <c r="M3">
-        <f>'Z 1745 d'!M3*Y!$C$18</f>
+        <f>'Z 1745 d'!M3*'Y Helic'!$C$18</f>
         <v>1.5436799999999999</v>
       </c>
       <c r="N3">
-        <f>'Z 1745 d'!N3*Y!$C$18</f>
+        <f>'Z 1745 d'!N3*'Y Helic'!$C$18</f>
         <v>1.4110199999999999</v>
       </c>
       <c r="O3">
-        <f>'Z 1745 d'!O3*Y!$C$18</f>
+        <f>'Z 1745 d'!O3*'Y Helic'!$C$18</f>
         <v>1.31454</v>
       </c>
     </row>
@@ -1315,59 +1315,59 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <f>'Z 1745 d'!B4*Y!$C$18</f>
+        <f>'Z 1745 d'!B4*'Y Helic'!$C$18</f>
         <v>3.2562000000000002</v>
       </c>
       <c r="C4">
-        <f>'Z 1745 d'!C4*Y!$C$18</f>
+        <f>'Z 1745 d'!C4*'Y Helic'!$C$18</f>
         <v>3.1476599999999997</v>
       </c>
       <c r="D4">
-        <f>'Z 1745 d'!D4*Y!$C$18</f>
+        <f>'Z 1745 d'!D4*'Y Helic'!$C$18</f>
         <v>3.0752999999999995</v>
       </c>
       <c r="E4">
-        <f>'Z 1745 d'!E4*Y!$C$18</f>
+        <f>'Z 1745 d'!E4*'Y Helic'!$C$18</f>
         <v>2.9426399999999999</v>
       </c>
       <c r="F4">
-        <f>'Z 1745 d'!F4*Y!$C$18</f>
+        <f>'Z 1745 d'!F4*'Y Helic'!$C$18</f>
         <v>2.8461599999999998</v>
       </c>
       <c r="G4">
-        <f>'Z 1745 d'!G4*Y!$C$18</f>
+        <f>'Z 1745 d'!G4*'Y Helic'!$C$18</f>
         <v>2.7134999999999998</v>
       </c>
       <c r="H4">
-        <f>'Z 1745 d'!H4*Y!$C$18</f>
+        <f>'Z 1745 d'!H4*'Y Helic'!$C$18</f>
         <v>2.6049600000000002</v>
       </c>
       <c r="I4">
-        <f>'Z 1745 d'!I4*Y!$C$18</f>
+        <f>'Z 1745 d'!I4*'Y Helic'!$C$18</f>
         <v>2.4240599999999999</v>
       </c>
       <c r="J4">
-        <f>'Z 1745 d'!J4*Y!$C$18</f>
+        <f>'Z 1745 d'!J4*'Y Helic'!$C$18</f>
         <v>2.2069800000000002</v>
       </c>
       <c r="K4">
-        <f>'Z 1745 d'!K4*Y!$C$18</f>
+        <f>'Z 1745 d'!K4*'Y Helic'!$C$18</f>
         <v>2.0984400000000001</v>
       </c>
       <c r="L4">
-        <f>'Z 1745 d'!L4*Y!$C$18</f>
+        <f>'Z 1745 d'!L4*'Y Helic'!$C$18</f>
         <v>1.9416600000000002</v>
       </c>
       <c r="M4">
-        <f>'Z 1745 d'!M4*Y!$C$18</f>
+        <f>'Z 1745 d'!M4*'Y Helic'!$C$18</f>
         <v>1.7245799999999998</v>
       </c>
       <c r="N4">
-        <f>'Z 1745 d'!N4*Y!$C$18</f>
+        <f>'Z 1745 d'!N4*'Y Helic'!$C$18</f>
         <v>1.5557399999999999</v>
       </c>
       <c r="O4">
-        <f>'Z 1745 d'!O4*Y!$C$18</f>
+        <f>'Z 1745 d'!O4*'Y Helic'!$C$18</f>
         <v>1.4230799999999999</v>
       </c>
     </row>
@@ -1377,59 +1377,59 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <f>'Z 1745 d'!B5*Y!$C$18</f>
+        <f>'Z 1745 d'!B5*'Y Helic'!$C$18</f>
         <v>4.0400999999999998</v>
       </c>
       <c r="C5">
-        <f>'Z 1745 d'!C5*Y!$C$18</f>
+        <f>'Z 1745 d'!C5*'Y Helic'!$C$18</f>
         <v>3.9074400000000002</v>
       </c>
       <c r="D5">
-        <f>'Z 1745 d'!D5*Y!$C$18</f>
+        <f>'Z 1745 d'!D5*'Y Helic'!$C$18</f>
         <v>3.83508</v>
       </c>
       <c r="E5">
-        <f>'Z 1745 d'!E5*Y!$C$18</f>
+        <f>'Z 1745 d'!E5*'Y Helic'!$C$18</f>
         <v>3.6179999999999999</v>
       </c>
       <c r="F5">
-        <f>'Z 1745 d'!F5*Y!$C$18</f>
+        <f>'Z 1745 d'!F5*'Y Helic'!$C$18</f>
         <v>3.4973999999999998</v>
       </c>
       <c r="G5">
-        <f>'Z 1745 d'!G5*Y!$C$18</f>
+        <f>'Z 1745 d'!G5*'Y Helic'!$C$18</f>
         <v>3.2562000000000002</v>
       </c>
       <c r="H5">
-        <f>'Z 1745 d'!H5*Y!$C$18</f>
+        <f>'Z 1745 d'!H5*'Y Helic'!$C$18</f>
         <v>3.0873599999999999</v>
       </c>
       <c r="I5">
-        <f>'Z 1745 d'!I5*Y!$C$18</f>
+        <f>'Z 1745 d'!I5*'Y Helic'!$C$18</f>
         <v>2.8823400000000001</v>
       </c>
       <c r="J5">
-        <f>'Z 1745 d'!J5*Y!$C$18</f>
+        <f>'Z 1745 d'!J5*'Y Helic'!$C$18</f>
         <v>2.6049600000000002</v>
       </c>
       <c r="K5">
-        <f>'Z 1745 d'!K5*Y!$C$18</f>
+        <f>'Z 1745 d'!K5*'Y Helic'!$C$18</f>
         <v>2.4481799999999998</v>
       </c>
       <c r="L5">
-        <f>'Z 1745 d'!L5*Y!$C$18</f>
+        <f>'Z 1745 d'!L5*'Y Helic'!$C$18</f>
         <v>2.1949200000000002</v>
       </c>
       <c r="M5">
-        <f>'Z 1745 d'!M5*Y!$C$18</f>
+        <f>'Z 1745 d'!M5*'Y Helic'!$C$18</f>
         <v>1.9296</v>
       </c>
       <c r="N5">
-        <f>'Z 1745 d'!N5*Y!$C$18</f>
+        <f>'Z 1745 d'!N5*'Y Helic'!$C$18</f>
         <v>1.7245799999999998</v>
       </c>
       <c r="O5">
-        <f>'Z 1745 d'!O5*Y!$C$18</f>
+        <f>'Z 1745 d'!O5*'Y Helic'!$C$18</f>
         <v>1.53162</v>
       </c>
     </row>
@@ -1439,59 +1439,59 @@
         <v>26</v>
       </c>
       <c r="B6">
-        <f>'Z 1745 d'!B6*Y!$C$18</f>
+        <f>'Z 1745 d'!B6*'Y Helic'!$C$18</f>
         <v>4.9445999999999994</v>
       </c>
       <c r="C6">
-        <f>'Z 1745 d'!C6*Y!$C$18</f>
+        <f>'Z 1745 d'!C6*'Y Helic'!$C$18</f>
         <v>4.7033999999999994</v>
       </c>
       <c r="D6">
-        <f>'Z 1745 d'!D6*Y!$C$18</f>
+        <f>'Z 1745 d'!D6*'Y Helic'!$C$18</f>
         <v>4.5827999999999998</v>
       </c>
       <c r="E6">
-        <f>'Z 1745 d'!E6*Y!$C$18</f>
+        <f>'Z 1745 d'!E6*'Y Helic'!$C$18</f>
         <v>4.3174799999999998</v>
       </c>
       <c r="F6">
-        <f>'Z 1745 d'!F6*Y!$C$18</f>
+        <f>'Z 1745 d'!F6*'Y Helic'!$C$18</f>
         <v>4.1245199999999995</v>
       </c>
       <c r="G6">
-        <f>'Z 1745 d'!G6*Y!$C$18</f>
+        <f>'Z 1745 d'!G6*'Y Helic'!$C$18</f>
         <v>3.7868400000000002</v>
       </c>
       <c r="H6">
-        <f>'Z 1745 d'!H6*Y!$C$18</f>
+        <f>'Z 1745 d'!H6*'Y Helic'!$C$18</f>
         <v>3.56976</v>
       </c>
       <c r="I6">
-        <f>'Z 1745 d'!I6*Y!$C$18</f>
+        <f>'Z 1745 d'!I6*'Y Helic'!$C$18</f>
         <v>3.30444</v>
       </c>
       <c r="J6">
-        <f>'Z 1745 d'!J6*Y!$C$18</f>
+        <f>'Z 1745 d'!J6*'Y Helic'!$C$18</f>
         <v>2.9426399999999999</v>
       </c>
       <c r="K6">
-        <f>'Z 1745 d'!K6*Y!$C$18</f>
+        <f>'Z 1745 d'!K6*'Y Helic'!$C$18</f>
         <v>2.7617400000000001</v>
       </c>
       <c r="L6">
-        <f>'Z 1745 d'!L6*Y!$C$18</f>
+        <f>'Z 1745 d'!L6*'Y Helic'!$C$18</f>
         <v>2.4361199999999998</v>
       </c>
       <c r="M6">
-        <f>'Z 1745 d'!M6*Y!$C$18</f>
+        <f>'Z 1745 d'!M6*'Y Helic'!$C$18</f>
         <v>2.0863800000000001</v>
       </c>
       <c r="N6">
-        <f>'Z 1745 d'!N6*Y!$C$18</f>
+        <f>'Z 1745 d'!N6*'Y Helic'!$C$18</f>
         <v>1.85724</v>
       </c>
       <c r="O6">
-        <f>'Z 1745 d'!O6*Y!$C$18</f>
+        <f>'Z 1745 d'!O6*'Y Helic'!$C$18</f>
         <v>1.6642799999999998</v>
       </c>
     </row>
@@ -1501,59 +1501,59 @@
         <v>30</v>
       </c>
       <c r="B7">
-        <f>'Z 1745 d'!B7*Y!$C$18</f>
+        <f>'Z 1745 d'!B7*'Y Helic'!$C$18</f>
         <v>5.6561400000000006</v>
       </c>
       <c r="C7">
-        <f>'Z 1745 d'!C7*Y!$C$18</f>
+        <f>'Z 1745 d'!C7*'Y Helic'!$C$18</f>
         <v>5.3908199999999997</v>
       </c>
       <c r="D7">
-        <f>'Z 1745 d'!D7*Y!$C$18</f>
+        <f>'Z 1745 d'!D7*'Y Helic'!$C$18</f>
         <v>5.1496199999999996</v>
       </c>
       <c r="E7">
-        <f>'Z 1745 d'!E7*Y!$C$18</f>
+        <f>'Z 1745 d'!E7*'Y Helic'!$C$18</f>
         <v>4.7637</v>
       </c>
       <c r="F7">
-        <f>'Z 1745 d'!F7*Y!$C$18</f>
+        <f>'Z 1745 d'!F7*'Y Helic'!$C$18</f>
         <v>4.5345599999999999</v>
       </c>
       <c r="G7">
-        <f>'Z 1745 d'!G7*Y!$C$18</f>
+        <f>'Z 1745 d'!G7*'Y Helic'!$C$18</f>
         <v>4.1727600000000002</v>
       </c>
       <c r="H7">
-        <f>'Z 1745 d'!H7*Y!$C$18</f>
+        <f>'Z 1745 d'!H7*'Y Helic'!$C$18</f>
         <v>3.8833200000000003</v>
       </c>
       <c r="I7">
-        <f>'Z 1745 d'!I7*Y!$C$18</f>
+        <f>'Z 1745 d'!I7*'Y Helic'!$C$18</f>
         <v>3.5335800000000002</v>
       </c>
       <c r="J7">
-        <f>'Z 1745 d'!J7*Y!$C$18</f>
+        <f>'Z 1745 d'!J7*'Y Helic'!$C$18</f>
         <v>3.1476599999999997</v>
       </c>
       <c r="K7">
-        <f>'Z 1745 d'!K7*Y!$C$18</f>
+        <f>'Z 1745 d'!K7*'Y Helic'!$C$18</f>
         <v>2.9426399999999999</v>
       </c>
       <c r="L7">
-        <f>'Z 1745 d'!L7*Y!$C$18</f>
+        <f>'Z 1745 d'!L7*'Y Helic'!$C$18</f>
         <v>2.6170199999999997</v>
       </c>
       <c r="M7">
-        <f>'Z 1745 d'!M7*Y!$C$18</f>
+        <f>'Z 1745 d'!M7*'Y Helic'!$C$18</f>
         <v>2.2069800000000002</v>
       </c>
       <c r="N7">
-        <f>'Z 1745 d'!N7*Y!$C$18</f>
+        <f>'Z 1745 d'!N7*'Y Helic'!$C$18</f>
         <v>1.9296</v>
       </c>
       <c r="O7">
-        <f>'Z 1745 d'!O7*Y!$C$18</f>
+        <f>'Z 1745 d'!O7*'Y Helic'!$C$18</f>
         <v>1.7486999999999999</v>
       </c>
     </row>
@@ -1563,59 +1563,59 @@
         <v>40</v>
       </c>
       <c r="B8">
-        <f>'Z 1745 d'!B8*Y!$C$18</f>
+        <f>'Z 1745 d'!B8*'Y Helic'!$C$18</f>
         <v>6.9947999999999997</v>
       </c>
       <c r="C8">
-        <f>'Z 1745 d'!C8*Y!$C$18</f>
+        <f>'Z 1745 d'!C8*'Y Helic'!$C$18</f>
         <v>6.6088800000000001</v>
       </c>
       <c r="D8">
-        <f>'Z 1745 d'!D8*Y!$C$18</f>
+        <f>'Z 1745 d'!D8*'Y Helic'!$C$18</f>
         <v>6.2470799999999995</v>
       </c>
       <c r="E8">
-        <f>'Z 1745 d'!E8*Y!$C$18</f>
+        <f>'Z 1745 d'!E8*'Y Helic'!$C$18</f>
         <v>5.6923199999999996</v>
       </c>
       <c r="F8">
-        <f>'Z 1745 d'!F8*Y!$C$18</f>
+        <f>'Z 1745 d'!F8*'Y Helic'!$C$18</f>
         <v>5.3546400000000007</v>
       </c>
       <c r="G8">
-        <f>'Z 1745 d'!G8*Y!$C$18</f>
+        <f>'Z 1745 d'!G8*'Y Helic'!$C$18</f>
         <v>4.7998799999999999</v>
       </c>
       <c r="H8">
-        <f>'Z 1745 d'!H8*Y!$C$18</f>
+        <f>'Z 1745 d'!H8*'Y Helic'!$C$18</f>
         <v>4.4622000000000002</v>
       </c>
       <c r="I8">
-        <f>'Z 1745 d'!I8*Y!$C$18</f>
+        <f>'Z 1745 d'!I8*'Y Helic'!$C$18</f>
         <v>4.0280399999999998</v>
       </c>
       <c r="J8">
-        <f>'Z 1745 d'!J8*Y!$C$18</f>
+        <f>'Z 1745 d'!J8*'Y Helic'!$C$18</f>
         <v>3.5215199999999998</v>
       </c>
       <c r="K8">
-        <f>'Z 1745 d'!K8*Y!$C$18</f>
+        <f>'Z 1745 d'!K8*'Y Helic'!$C$18</f>
         <v>3.2803200000000001</v>
       </c>
       <c r="L8">
-        <f>'Z 1745 d'!L8*Y!$C$18</f>
+        <f>'Z 1745 d'!L8*'Y Helic'!$C$18</f>
         <v>2.8702799999999997</v>
       </c>
       <c r="M8">
-        <f>'Z 1745 d'!M8*Y!$C$18</f>
+        <f>'Z 1745 d'!M8*'Y Helic'!$C$18</f>
         <v>2.4119999999999999</v>
       </c>
       <c r="N8">
-        <f>'Z 1745 d'!N8*Y!$C$18</f>
+        <f>'Z 1745 d'!N8*'Y Helic'!$C$18</f>
         <v>2.0743199999999997</v>
       </c>
       <c r="O8">
-        <f>'Z 1745 d'!O8*Y!$C$18</f>
+        <f>'Z 1745 d'!O8*'Y Helic'!$C$18</f>
         <v>1.8331199999999999</v>
       </c>
     </row>
@@ -1625,59 +1625,59 @@
         <v>50</v>
       </c>
       <c r="B9">
-        <f>'Z 1745 d'!B9*Y!$C$18</f>
+        <f>'Z 1745 d'!B9*'Y Helic'!$C$18</f>
         <v>8.1284399999999994</v>
       </c>
       <c r="C9">
-        <f>'Z 1745 d'!C9*Y!$C$18</f>
+        <f>'Z 1745 d'!C9*'Y Helic'!$C$18</f>
         <v>7.5977999999999994</v>
       </c>
       <c r="D9">
-        <f>'Z 1745 d'!D9*Y!$C$18</f>
+        <f>'Z 1745 d'!D9*'Y Helic'!$C$18</f>
         <v>7.2359999999999998</v>
       </c>
       <c r="E9">
-        <f>'Z 1745 d'!E9*Y!$C$18</f>
+        <f>'Z 1745 d'!E9*'Y Helic'!$C$18</f>
         <v>6.5244600000000004</v>
       </c>
       <c r="F9">
-        <f>'Z 1745 d'!F9*Y!$C$18</f>
+        <f>'Z 1745 d'!F9*'Y Helic'!$C$18</f>
         <v>5.9576400000000005</v>
       </c>
       <c r="G9">
-        <f>'Z 1745 d'!G9*Y!$C$18</f>
+        <f>'Z 1745 d'!G9*'Y Helic'!$C$18</f>
         <v>5.3908199999999997</v>
       </c>
       <c r="H9">
-        <f>'Z 1745 d'!H9*Y!$C$18</f>
+        <f>'Z 1745 d'!H9*'Y Helic'!$C$18</f>
         <v>5.0410799999999991</v>
       </c>
       <c r="I9">
-        <f>'Z 1745 d'!I9*Y!$C$18</f>
+        <f>'Z 1745 d'!I9*'Y Helic'!$C$18</f>
         <v>4.4622000000000002</v>
       </c>
       <c r="J9">
-        <f>'Z 1745 d'!J9*Y!$C$18</f>
+        <f>'Z 1745 d'!J9*'Y Helic'!$C$18</f>
         <v>3.8592</v>
       </c>
       <c r="K9">
-        <f>'Z 1745 d'!K9*Y!$C$18</f>
+        <f>'Z 1745 d'!K9*'Y Helic'!$C$18</f>
         <v>3.5456399999999997</v>
       </c>
       <c r="L9">
-        <f>'Z 1745 d'!L9*Y!$C$18</f>
+        <f>'Z 1745 d'!L9*'Y Helic'!$C$18</f>
         <v>3.0752999999999995</v>
       </c>
       <c r="M9">
-        <f>'Z 1745 d'!M9*Y!$C$18</f>
+        <f>'Z 1745 d'!M9*'Y Helic'!$C$18</f>
         <v>2.5808400000000002</v>
       </c>
       <c r="N9">
-        <f>'Z 1745 d'!N9*Y!$C$18</f>
+        <f>'Z 1745 d'!N9*'Y Helic'!$C$18</f>
         <v>2.1828599999999998</v>
       </c>
       <c r="O9">
-        <f>'Z 1745 d'!O9*Y!$C$18</f>
+        <f>'Z 1745 d'!O9*'Y Helic'!$C$18</f>
         <v>1.9054800000000001</v>
       </c>
     </row>
@@ -1687,59 +1687,59 @@
         <v>60</v>
       </c>
       <c r="B10">
-        <f>'Z 1745 d'!B10*Y!$C$18</f>
+        <f>'Z 1745 d'!B10*'Y Helic'!$C$18</f>
         <v>8.9002800000000004</v>
       </c>
       <c r="C10">
-        <f>'Z 1745 d'!C10*Y!$C$18</f>
+        <f>'Z 1745 d'!C10*'Y Helic'!$C$18</f>
         <v>8.2369799999999991</v>
       </c>
       <c r="D10">
-        <f>'Z 1745 d'!D10*Y!$C$18</f>
+        <f>'Z 1745 d'!D10*'Y Helic'!$C$18</f>
         <v>7.8389999999999995</v>
       </c>
       <c r="E10">
-        <f>'Z 1745 d'!E10*Y!$C$18</f>
+        <f>'Z 1745 d'!E10*'Y Helic'!$C$18</f>
         <v>7.0309799999999996</v>
       </c>
       <c r="F10">
-        <f>'Z 1745 d'!F10*Y!$C$18</f>
+        <f>'Z 1745 d'!F10*'Y Helic'!$C$18</f>
         <v>6.4520999999999997</v>
       </c>
       <c r="G10">
-        <f>'Z 1745 d'!G10*Y!$C$18</f>
+        <f>'Z 1745 d'!G10*'Y Helic'!$C$18</f>
         <v>5.7405599999999994</v>
       </c>
       <c r="H10">
-        <f>'Z 1745 d'!H10*Y!$C$18</f>
+        <f>'Z 1745 d'!H10*'Y Helic'!$C$18</f>
         <v>5.2943399999999992</v>
       </c>
       <c r="I10">
-        <f>'Z 1745 d'!I10*Y!$C$18</f>
+        <f>'Z 1745 d'!I10*'Y Helic'!$C$18</f>
         <v>4.7395800000000001</v>
       </c>
       <c r="J10">
-        <f>'Z 1745 d'!J10*Y!$C$18</f>
+        <f>'Z 1745 d'!J10*'Y Helic'!$C$18</f>
         <v>4.0762799999999997</v>
       </c>
       <c r="K10">
-        <f>'Z 1745 d'!K10*Y!$C$18</f>
+        <f>'Z 1745 d'!K10*'Y Helic'!$C$18</f>
         <v>3.7627199999999998</v>
       </c>
       <c r="L10">
-        <f>'Z 1745 d'!L10*Y!$C$18</f>
+        <f>'Z 1745 d'!L10*'Y Helic'!$C$18</f>
         <v>3.2079599999999999</v>
       </c>
       <c r="M10">
-        <f>'Z 1745 d'!M10*Y!$C$18</f>
+        <f>'Z 1745 d'!M10*'Y Helic'!$C$18</f>
         <v>2.6773200000000004</v>
       </c>
       <c r="N10">
-        <f>'Z 1745 d'!N10*Y!$C$18</f>
+        <f>'Z 1745 d'!N10*'Y Helic'!$C$18</f>
         <v>2.25522</v>
       </c>
       <c r="O10">
-        <f>'Z 1745 d'!O10*Y!$C$18</f>
+        <f>'Z 1745 d'!O10*'Y Helic'!$C$18</f>
         <v>1.9778399999999998</v>
       </c>
     </row>
@@ -1749,59 +1749,59 @@
         <v>80</v>
       </c>
       <c r="B11">
-        <f>'Z 1745 d'!B11*Y!$C$18</f>
+        <f>'Z 1745 d'!B11*'Y Helic'!$C$18</f>
         <v>10.72134</v>
       </c>
       <c r="C11">
-        <f>'Z 1745 d'!C11*Y!$C$18</f>
+        <f>'Z 1745 d'!C11*'Y Helic'!$C$18</f>
         <v>9.5756399999999999</v>
       </c>
       <c r="D11">
-        <f>'Z 1745 d'!D11*Y!$C$18</f>
+        <f>'Z 1745 d'!D11*'Y Helic'!$C$18</f>
         <v>9.0449999999999999</v>
       </c>
       <c r="E11">
-        <f>'Z 1745 d'!E11*Y!$C$18</f>
+        <f>'Z 1745 d'!E11*'Y Helic'!$C$18</f>
         <v>8.0801999999999996</v>
       </c>
       <c r="F11">
-        <f>'Z 1745 d'!F11*Y!$C$18</f>
+        <f>'Z 1745 d'!F11*'Y Helic'!$C$18</f>
         <v>7.4169</v>
       </c>
       <c r="G11">
-        <f>'Z 1745 d'!G11*Y!$C$18</f>
+        <f>'Z 1745 d'!G11*'Y Helic'!$C$18</f>
         <v>6.5365199999999994</v>
       </c>
       <c r="H11">
-        <f>'Z 1745 d'!H11*Y!$C$18</f>
+        <f>'Z 1745 d'!H11*'Y Helic'!$C$18</f>
         <v>5.9576400000000005</v>
       </c>
       <c r="I11">
-        <f>'Z 1745 d'!I11*Y!$C$18</f>
+        <f>'Z 1745 d'!I11*'Y Helic'!$C$18</f>
         <v>5.3305199999999999</v>
       </c>
       <c r="J11">
-        <f>'Z 1745 d'!J11*Y!$C$18</f>
+        <f>'Z 1745 d'!J11*'Y Helic'!$C$18</f>
         <v>4.51044</v>
       </c>
       <c r="K11">
-        <f>'Z 1745 d'!K11*Y!$C$18</f>
+        <f>'Z 1745 d'!K11*'Y Helic'!$C$18</f>
         <v>4.1124600000000004</v>
       </c>
       <c r="L11">
-        <f>'Z 1745 d'!L11*Y!$C$18</f>
+        <f>'Z 1745 d'!L11*'Y Helic'!$C$18</f>
         <v>3.46122</v>
       </c>
       <c r="M11">
-        <f>'Z 1745 d'!M11*Y!$C$18</f>
+        <f>'Z 1745 d'!M11*'Y Helic'!$C$18</f>
         <v>2.8461599999999998</v>
       </c>
       <c r="N11">
-        <f>'Z 1745 d'!N11*Y!$C$18</f>
+        <f>'Z 1745 d'!N11*'Y Helic'!$C$18</f>
         <v>2.38788</v>
       </c>
       <c r="O11">
-        <f>'Z 1745 d'!O11*Y!$C$18</f>
+        <f>'Z 1745 d'!O11*'Y Helic'!$C$18</f>
         <v>2.1105</v>
       </c>
     </row>
@@ -1811,59 +1811,59 @@
         <v>100</v>
       </c>
       <c r="B12">
-        <f>'Z 1745 d'!B12*Y!$C$18</f>
+        <f>'Z 1745 d'!B12*'Y Helic'!$C$18</f>
         <v>12.86802</v>
       </c>
       <c r="C12">
-        <f>'Z 1745 d'!C12*Y!$C$18</f>
+        <f>'Z 1745 d'!C12*'Y Helic'!$C$18</f>
         <v>11.16756</v>
       </c>
       <c r="D12">
-        <f>'Z 1745 d'!D12*Y!$C$18</f>
+        <f>'Z 1745 d'!D12*'Y Helic'!$C$18</f>
         <v>10.1304</v>
       </c>
       <c r="E12">
-        <f>'Z 1745 d'!E12*Y!$C$18</f>
+        <f>'Z 1745 d'!E12*'Y Helic'!$C$18</f>
         <v>8.8640999999999988</v>
       </c>
       <c r="F12">
-        <f>'Z 1745 d'!F12*Y!$C$18</f>
+        <f>'Z 1745 d'!F12*'Y Helic'!$C$18</f>
         <v>8.0922599999999996</v>
       </c>
       <c r="G12">
-        <f>'Z 1745 d'!G12*Y!$C$18</f>
+        <f>'Z 1745 d'!G12*'Y Helic'!$C$18</f>
         <v>7.0912799999999994</v>
       </c>
       <c r="H12">
-        <f>'Z 1745 d'!H12*Y!$C$18</f>
+        <f>'Z 1745 d'!H12*'Y Helic'!$C$18</f>
         <v>6.4641600000000006</v>
       </c>
       <c r="I12">
-        <f>'Z 1745 d'!I12*Y!$C$18</f>
+        <f>'Z 1745 d'!I12*'Y Helic'!$C$18</f>
         <v>5.6320199999999998</v>
       </c>
       <c r="J12">
-        <f>'Z 1745 d'!J12*Y!$C$18</f>
+        <f>'Z 1745 d'!J12*'Y Helic'!$C$18</f>
         <v>4.7516400000000001</v>
       </c>
       <c r="K12">
-        <f>'Z 1745 d'!K12*Y!$C$18</f>
+        <f>'Z 1745 d'!K12*'Y Helic'!$C$18</f>
         <v>4.3415999999999997</v>
       </c>
       <c r="L12">
-        <f>'Z 1745 d'!L12*Y!$C$18</f>
+        <f>'Z 1745 d'!L12*'Y Helic'!$C$18</f>
         <v>3.58182</v>
       </c>
       <c r="M12">
-        <f>'Z 1745 d'!M12*Y!$C$18</f>
+        <f>'Z 1745 d'!M12*'Y Helic'!$C$18</f>
         <v>2.93058</v>
       </c>
       <c r="N12">
-        <f>'Z 1745 d'!N12*Y!$C$18</f>
+        <f>'Z 1745 d'!N12*'Y Helic'!$C$18</f>
         <v>2.4722999999999997</v>
       </c>
       <c r="O12">
-        <f>'Z 1745 d'!O12*Y!$C$18</f>
+        <f>'Z 1745 d'!O12*'Y Helic'!$C$18</f>
         <v>2.1466799999999999</v>
       </c>
     </row>
@@ -1876,55 +1876,55 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>'Z 1745 d'!C13*Y!$C$18</f>
+        <f>'Z 1745 d'!C13*'Y Helic'!$C$18</f>
         <v>13.627800000000001</v>
       </c>
       <c r="D13">
-        <f>'Z 1745 d'!D13*Y!$C$18</f>
+        <f>'Z 1745 d'!D13*'Y Helic'!$C$18</f>
         <v>12.059999999999999</v>
       </c>
       <c r="E13">
-        <f>'Z 1745 d'!E13*Y!$C$18</f>
+        <f>'Z 1745 d'!E13*'Y Helic'!$C$18</f>
         <v>10.15452</v>
       </c>
       <c r="F13">
-        <f>'Z 1745 d'!F13*Y!$C$18</f>
+        <f>'Z 1745 d'!F13*'Y Helic'!$C$18</f>
         <v>9.0449999999999999</v>
       </c>
       <c r="G13">
-        <f>'Z 1745 d'!G13*Y!$C$18</f>
+        <f>'Z 1745 d'!G13*'Y Helic'!$C$18</f>
         <v>7.8389999999999995</v>
       </c>
       <c r="H13">
-        <f>'Z 1745 d'!H13*Y!$C$18</f>
+        <f>'Z 1745 d'!H13*'Y Helic'!$C$18</f>
         <v>7.1395200000000001</v>
       </c>
       <c r="I13">
-        <f>'Z 1745 d'!I13*Y!$C$18</f>
+        <f>'Z 1745 d'!I13*'Y Helic'!$C$18</f>
         <v>6.11442</v>
       </c>
       <c r="J13">
-        <f>'Z 1745 d'!J13*Y!$C$18</f>
+        <f>'Z 1745 d'!J13*'Y Helic'!$C$18</f>
         <v>5.1134399999999998</v>
       </c>
       <c r="K13">
-        <f>'Z 1745 d'!K13*Y!$C$18</f>
+        <f>'Z 1745 d'!K13*'Y Helic'!$C$18</f>
         <v>4.6310399999999996</v>
       </c>
       <c r="L13">
-        <f>'Z 1745 d'!L13*Y!$C$18</f>
+        <f>'Z 1745 d'!L13*'Y Helic'!$C$18</f>
         <v>3.8230199999999996</v>
       </c>
       <c r="M13">
-        <f>'Z 1745 d'!M13*Y!$C$18</f>
+        <f>'Z 1745 d'!M13*'Y Helic'!$C$18</f>
         <v>3.03912</v>
       </c>
       <c r="N13">
-        <f>'Z 1745 d'!N13*Y!$C$18</f>
+        <f>'Z 1745 d'!N13*'Y Helic'!$C$18</f>
         <v>2.5808400000000002</v>
       </c>
       <c r="O13">
-        <f>'Z 1745 d'!O13*Y!$C$18</f>
+        <f>'Z 1745 d'!O13*'Y Helic'!$C$18</f>
         <v>2.2190400000000001</v>
       </c>
     </row>
@@ -1940,51 +1940,51 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <f>'Z 1745 d'!D14*Y!$C$18</f>
+        <f>'Z 1745 d'!D14*'Y Helic'!$C$18</f>
         <v>13.507199999999999</v>
       </c>
       <c r="E14">
-        <f>'Z 1745 d'!E14*Y!$C$18</f>
+        <f>'Z 1745 d'!E14*'Y Helic'!$C$18</f>
         <v>11.05902</v>
       </c>
       <c r="F14">
-        <f>'Z 1745 d'!F14*Y!$C$18</f>
+        <f>'Z 1745 d'!F14*'Y Helic'!$C$18</f>
         <v>9.6479999999999997</v>
       </c>
       <c r="G14">
-        <f>'Z 1745 d'!G14*Y!$C$18</f>
+        <f>'Z 1745 d'!G14*'Y Helic'!$C$18</f>
         <v>8.2972799999999989</v>
       </c>
       <c r="H14">
-        <f>'Z 1745 d'!H14*Y!$C$18</f>
+        <f>'Z 1745 d'!H14*'Y Helic'!$C$18</f>
         <v>7.4771999999999998</v>
       </c>
       <c r="I14">
-        <f>'Z 1745 d'!I14*Y!$C$18</f>
+        <f>'Z 1745 d'!I14*'Y Helic'!$C$18</f>
         <v>6.4279799999999998</v>
       </c>
       <c r="J14">
-        <f>'Z 1745 d'!J14*Y!$C$18</f>
+        <f>'Z 1745 d'!J14*'Y Helic'!$C$18</f>
         <v>5.2702200000000001</v>
       </c>
       <c r="K14">
-        <f>'Z 1745 d'!K14*Y!$C$18</f>
+        <f>'Z 1745 d'!K14*'Y Helic'!$C$18</f>
         <v>4.77576</v>
       </c>
       <c r="L14">
-        <f>'Z 1745 d'!L14*Y!$C$18</f>
+        <f>'Z 1745 d'!L14*'Y Helic'!$C$18</f>
         <v>3.9194999999999998</v>
       </c>
       <c r="M14">
-        <f>'Z 1745 d'!M14*Y!$C$18</f>
+        <f>'Z 1745 d'!M14*'Y Helic'!$C$18</f>
         <v>3.2320800000000003</v>
       </c>
       <c r="N14">
-        <f>'Z 1745 d'!N14*Y!$C$18</f>
+        <f>'Z 1745 d'!N14*'Y Helic'!$C$18</f>
         <v>2.64114</v>
       </c>
       <c r="O14">
-        <f>'Z 1745 d'!O14*Y!$C$18</f>
+        <f>'Z 1745 d'!O14*'Y Helic'!$C$18</f>
         <v>2.26728</v>
       </c>
     </row>
@@ -2003,53 +2003,798 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <f>'Z 1745 d'!E15*Y!$C$18</f>
+        <f>'Z 1745 d'!E15*'Y Helic'!$C$18</f>
         <v>12.7233</v>
       </c>
       <c r="F15">
-        <f>'Z 1745 d'!F15*Y!$C$18</f>
+        <f>'Z 1745 d'!F15*'Y Helic'!$C$18</f>
         <v>10.986659999999999</v>
       </c>
       <c r="G15">
-        <f>'Z 1745 d'!G15*Y!$C$18</f>
+        <f>'Z 1745 d'!G15*'Y Helic'!$C$18</f>
         <v>9.02088</v>
       </c>
       <c r="H15">
-        <f>'Z 1745 d'!H15*Y!$C$18</f>
+        <f>'Z 1745 d'!H15*'Y Helic'!$C$18</f>
         <v>8.0440199999999997</v>
       </c>
       <c r="I15">
-        <f>'Z 1745 d'!I15*Y!$C$18</f>
+        <f>'Z 1745 d'!I15*'Y Helic'!$C$18</f>
         <v>6.8500799999999993</v>
       </c>
       <c r="J15">
-        <f>'Z 1745 d'!J15*Y!$C$18</f>
+        <f>'Z 1745 d'!J15*'Y Helic'!$C$18</f>
         <v>5.58378</v>
       </c>
       <c r="K15">
-        <f>'Z 1745 d'!K15*Y!$C$18</f>
+        <f>'Z 1745 d'!K15*'Y Helic'!$C$18</f>
         <v>4.9928399999999993</v>
       </c>
       <c r="L15">
-        <f>'Z 1745 d'!L15*Y!$C$18</f>
+        <f>'Z 1745 d'!L15*'Y Helic'!$C$18</f>
         <v>4.0400999999999998</v>
       </c>
       <c r="M15">
-        <f>'Z 1745 d'!M15*Y!$C$18</f>
+        <f>'Z 1745 d'!M15*'Y Helic'!$C$18</f>
         <v>3.2441399999999998</v>
       </c>
       <c r="N15">
-        <f>'Z 1745 d'!N15*Y!$C$18</f>
+        <f>'Z 1745 d'!N15*'Y Helic'!$C$18</f>
         <v>2.7255599999999998</v>
       </c>
       <c r="O15">
-        <f>'Z 1745 d'!O15*Y!$C$18</f>
+        <f>'Z 1745 d'!O15*'Y Helic'!$C$18</f>
         <v>2.3396399999999997</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>1.206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A84FA60F-B039-4785-A1CC-4FAE71DDEB4A}">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <f>'Z 1745 d'!B1</f>
+        <v>400</v>
+      </c>
+      <c r="C1">
+        <f>'Z 1745 d'!C1</f>
+        <v>200</v>
+      </c>
+      <c r="D1">
+        <f>'Z 1745 d'!D1</f>
+        <v>150</v>
+      </c>
+      <c r="E1">
+        <f>'Z 1745 d'!E1</f>
+        <v>100</v>
+      </c>
+      <c r="F1">
+        <f>'Z 1745 d'!F1</f>
+        <v>80</v>
+      </c>
+      <c r="G1">
+        <f>'Z 1745 d'!G1</f>
+        <v>60</v>
+      </c>
+      <c r="H1">
+        <f>'Z 1745 d'!H1</f>
+        <v>50</v>
+      </c>
+      <c r="I1">
+        <f>'Z 1745 d'!I1</f>
+        <v>40</v>
+      </c>
+      <c r="J1">
+        <f>'Z 1745 d'!J1</f>
+        <v>30</v>
+      </c>
+      <c r="K1">
+        <f>'Z 1745 d'!K1</f>
+        <v>26</v>
+      </c>
+      <c r="L1">
+        <f>'Z 1745 d'!L1</f>
+        <v>20</v>
+      </c>
+      <c r="M1">
+        <f>'Z 1745 d'!M1</f>
+        <v>15</v>
+      </c>
+      <c r="N1">
+        <f>'Z 1745 d'!N1</f>
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <f>'Z 1745 d'!O1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f>'Z 1745 d'!A2</f>
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="C2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D2">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="E2">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="F2">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="G2">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="H2">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="I2">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="J2">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="K2">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="L2">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="M2">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="N2">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="O2">
+        <v>0.53300000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>'Z 1745 d'!A3</f>
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="C3">
+        <v>0.63</v>
+      </c>
+      <c r="D3">
+        <v>0.625</v>
+      </c>
+      <c r="E3">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="F3">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="G3">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="H3">
+        <v>0.6</v>
+      </c>
+      <c r="I3">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="J3">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="K3">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="L3">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="M3">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="N3">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="O3">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>'Z 1745 d'!A4</f>
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="C4">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="D4">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="E4">
+        <v>0.67</v>
+      </c>
+      <c r="F4">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="G4">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="H4">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="I4">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="J4">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="K4">
+        <v>0.626</v>
+      </c>
+      <c r="L4">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="M4">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="N4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="O4">
+        <v>0.56299999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f>'Z 1745 d'!A5</f>
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>0.75</v>
+      </c>
+      <c r="C5">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="E5">
+        <v>0.72</v>
+      </c>
+      <c r="F5">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="G5">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="H5">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="I5">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="J5">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="K5">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="L5">
+        <v>0.626</v>
+      </c>
+      <c r="M5">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="N5">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="O5">
+        <v>0.56200000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f>'Z 1745 d'!A6</f>
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>0.79</v>
+      </c>
+      <c r="C6">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="D6">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="E6">
+        <v>0.753</v>
+      </c>
+      <c r="F6">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="G6">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="H6">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="I6">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="J6">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="K6">
+        <v>0.627</v>
+      </c>
+      <c r="L6">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="M6">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="N6">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="O6">
+        <v>0.55100000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f>'Z 1745 d'!A7</f>
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="C7">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="D7">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="E7">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="F7">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H7">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="I7">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="J7">
+        <v>0.623</v>
+      </c>
+      <c r="K7">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="L7">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="M7">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="N7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O7">
+        <v>0.54300000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>'Z 1745 d'!A8</f>
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="C8">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="D8">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="E8">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="F8">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="G8">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="H8">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="I8">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="J8">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="K8">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="L8">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="M8">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="N8">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="O8">
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f>'Z 1745 d'!A9</f>
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>0.872</v>
+      </c>
+      <c r="C9">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="D9">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="F9">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="G9">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="H9">
+        <v>0.752</v>
+      </c>
+      <c r="I9">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="J9">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="K9">
+        <v>0.62</v>
+      </c>
+      <c r="L9">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="M9">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="N9">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="O9">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f>'Z 1745 d'!A10</f>
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="E10">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="F10">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="G10">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="H10">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="I10">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="J10">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="K10">
+        <v>0.63</v>
+      </c>
+      <c r="L10">
+        <v>0.59</v>
+      </c>
+      <c r="M10">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="N10">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="O10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f>'Z 1745 d'!A11</f>
+        <v>80</v>
+      </c>
+      <c r="B11">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="C11">
+        <v>0.875</v>
+      </c>
+      <c r="D11">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="E11">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="F11">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="G11">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="H11">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="I11">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="J11">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="K11">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="L11">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="M11">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="N11">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="O11">
+        <v>0.51100000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>'Z 1745 d'!A12</f>
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="C12">
+        <v>0.875</v>
+      </c>
+      <c r="D12">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.84</v>
+      </c>
+      <c r="F12">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="G12">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="H12">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="I12">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="J12">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="K12">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="L12">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="M12">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="N12">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="O12">
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f>'Z 1745 d'!A13</f>
+        <v>150</v>
+      </c>
+      <c r="B13">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="C13">
+        <v>0.87</v>
+      </c>
+      <c r="D13">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="E13">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="F13">
+        <v>0.82</v>
+      </c>
+      <c r="G13">
+        <v>0.78</v>
+      </c>
+      <c r="H13">
+        <v>0.77</v>
+      </c>
+      <c r="I13">
+        <v>0.74</v>
+      </c>
+      <c r="J13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="K13">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="L13">
+        <v>0.628</v>
+      </c>
+      <c r="M13">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="N13">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="O13">
+        <v>0.53300000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f>'Z 1745 d'!A14</f>
+        <v>200</v>
+      </c>
+      <c r="B14">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="C14">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="D14">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="E14">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="F14">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="G14">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="H14">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="I14">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="J14">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="K14">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="L14">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="M14">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="N14">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="O14">
+        <v>0.53700000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f>'Z 1745 d'!A15</f>
+        <v>400</v>
+      </c>
+      <c r="B15">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="C15">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.85</v>
+      </c>
+      <c r="E15">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="F15">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="G15">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="H15">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="I15">
+        <v>0.747</v>
+      </c>
+      <c r="J15">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="K15">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="L15">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="M15">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="N15">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="O15">
+        <v>0.55000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>